<commit_message>
Remove Ef for Asset Queries
</commit_message>
<xml_diff>
--- a/WebClient/ResultFiles/IRFC_SITE_SF1044.xlsx
+++ b/WebClient/ResultFiles/IRFC_SITE_SF1044.xlsx
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="154">
   <si>
     <t>SF1044</t>
   </si>
@@ -572,13 +572,13 @@
     </r>
   </si>
   <si>
-    <t>41.74</t>
-  </si>
-  <si>
-    <t>46.73</t>
-  </si>
-  <si>
-    <t>47.48</t>
+    <t>44.17</t>
+  </si>
+  <si>
+    <t>46.94</t>
+  </si>
+  <si>
+    <t>47.69</t>
   </si>
   <si>
     <t>TMA Type New</t>
@@ -717,7 +717,7 @@
     <t xml:space="preserve">8 </t>
   </si>
   <si>
-    <t xml:space="preserve"> 7 9</t>
+    <t xml:space="preserve"> 9 7</t>
   </si>
   <si>
     <t>7</t>
@@ -1033,7 +1033,7 @@
     <t>DateTime</t>
   </si>
   <si>
-    <t>2021-07-01</t>
+    <t>2021-07-06</t>
   </si>
   <si>
     <t>SiteName</t>
@@ -1123,19 +1123,16 @@
     <t>RF_Engineer</t>
   </si>
   <si>
-    <t>Victor Slavchev</t>
+    <t>mementa.velinova@gmail.com</t>
   </si>
   <si>
     <t>Mobile</t>
   </si>
   <si>
-    <t>0878500407</t>
+    <t>+359878500157</t>
   </si>
   <si>
     <t>Email</t>
-  </si>
-  <si>
-    <t>victor.slavchev@vivacom.bg</t>
   </si>
   <si>
     <t>APM30</t>
@@ -3400,7 +3397,7 @@
         <v>147</v>
       </c>
       <c r="B21" s="99" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -4348,32 +4345,32 @@
     </row>
     <row r="3" ht="13.8">
       <c r="A3" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" ht="13.8">
       <c r="A4" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" ht="13.8">
       <c r="A5" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" ht="13.8">
       <c r="A6" s="24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" ht="13.8">
       <c r="A7" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" ht="13.8">
       <c r="A8" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -5310,19 +5307,19 @@
         <v>0</v>
       </c>
       <c r="D33" s="19">
-        <v>49.35</v>
+        <v>49.832817797888154</v>
       </c>
       <c r="E33" s="19">
-        <v>52.56</v>
+        <v>50.560917449153713</v>
       </c>
       <c r="F33" s="19">
-        <v>47.029999999999994</v>
+        <v>47.2418124604762</v>
       </c>
       <c r="G33" s="19">
-        <v>52.56</v>
+        <v>50.560917449153713</v>
       </c>
       <c r="H33" s="19">
-        <v>47.029999999999994</v>
+        <v>47.2418124604762</v>
       </c>
       <c r="I33" s="19">
         <v>0</v>
@@ -6481,19 +6478,19 @@
         <v>0</v>
       </c>
       <c r="D33" s="19">
-        <v>49.35</v>
+        <v>49.832817797888154</v>
       </c>
       <c r="E33" s="19">
-        <v>52.67</v>
+        <v>50.670917449153713</v>
       </c>
       <c r="F33" s="19">
-        <v>47.029999999999994</v>
+        <v>47.2418124604762</v>
       </c>
       <c r="G33" s="19">
-        <v>52.67</v>
+        <v>50.670917449153713</v>
       </c>
       <c r="H33" s="19">
-        <v>47.029999999999994</v>
+        <v>47.2418124604762</v>
       </c>
       <c r="I33" s="19">
         <v>0</v>
@@ -7652,19 +7649,19 @@
         <v>0</v>
       </c>
       <c r="D33" s="19">
-        <v>49.35</v>
+        <v>49.832817797888154</v>
       </c>
       <c r="E33" s="19">
-        <v>52.67</v>
+        <v>50.670917449153713</v>
       </c>
       <c r="F33" s="19">
-        <v>47.029999999999994</v>
+        <v>47.2418124604762</v>
       </c>
       <c r="G33" s="19">
-        <v>52.67</v>
+        <v>50.670917449153713</v>
       </c>
       <c r="H33" s="19">
-        <v>47.029999999999994</v>
+        <v>47.2418124604762</v>
       </c>
       <c r="I33" s="19">
         <v>0</v>

</xml_diff>